<commit_message>
if to impf in demo_today.xlsx
</commit_message>
<xml_diff>
--- a/data/demo/demo_today.xlsx
+++ b/data/demo/demo_today.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aznarsig/Documents/Python/climada_python/data/demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeliestalhanske/python_projects/climada_python/data/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{06E713F1-4886-8347-ADA7-B75FFD6E7C01}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02D6A40-57DA-9944-897B-137BA654B587}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9800" yWindow="1580" windowWidth="27320" windowHeight="14820" tabRatio="766" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1480" yWindow="1580" windowWidth="27320" windowHeight="14820" tabRatio="766" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="assets" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,19 @@
     <sheet name="_measures_details" sheetId="5" r:id="rId6"/>
     <sheet name="_discounting_sheet" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1274,9 +1283,6 @@
     <t>cover</t>
   </si>
   <si>
-    <t>if_TC</t>
-  </si>
-  <si>
     <t>impact_fun_id</t>
   </si>
   <si>
@@ -1308,6 +1314,9 @@
   </si>
   <si>
     <t>peril_ID</t>
+  </si>
+  <si>
+    <t>impf_TC</t>
   </si>
 </sst>
 </file>
@@ -2092,7 +2101,7 @@
                 <a:cs typeface="SwissReSans"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="545681760"/>
@@ -2141,7 +2150,7 @@
                 <a:cs typeface="SwissReSans"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="545677200"/>
@@ -2188,7 +2197,7 @@
               <a:cs typeface="SwissReSans"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2221,7 +2230,7 @@
           <a:cs typeface="SwissReSans"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2681,7 +2690,7 @@
                 <a:cs typeface="SwissReSans"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="546681792"/>
@@ -2730,7 +2739,7 @@
                 <a:cs typeface="SwissReSans"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CH"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="546677232"/>
@@ -2777,7 +2786,7 @@
               <a:cs typeface="SwissReSans"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CH"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2810,7 +2819,7 @@
           <a:cs typeface="SwissReSans"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CH"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3258,7 +3267,7 @@
         <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="G1" s="20" t="s">
         <v>45</v>
@@ -4524,7 +4533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4538,25 +4547,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="24" t="s">
+      <c r="G1" s="26" t="s">
         <v>76</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>77</v>
       </c>
       <c r="H1" s="26" t="s">
         <v>1</v>
@@ -5094,10 +5103,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>79</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
@@ -5121,10 +5130,10 @@
         <v>56</v>
       </c>
       <c r="M1" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" s="32" t="s">
         <v>80</v>
-      </c>
-      <c r="N1" s="32" t="s">
-        <v>81</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>5</v>
@@ -5133,7 +5142,7 @@
         <v>6</v>
       </c>
       <c r="Q1" s="34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.15">
@@ -6372,7 +6381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>